<commit_message>
JS Applications - Remote databases - Book App
</commit_message>
<xml_diff>
--- a/JS Applications/JS-Hints.xlsx
+++ b/JS Applications/JS-Hints.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="UnitTesting" sheetId="1" r:id="rId1"/>
+    <sheet name="REST-Services-And-AJAX" sheetId="2" r:id="rId2"/>
+    <sheet name="ASYNCHRONOUS PROGRAMMING" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>browser testing</t>
   </si>
@@ -94,11 +96,67 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>XMLHttpRequest – Standard API for AJAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;button id = "load"&gt;Load Repos&lt;/button&gt;
+&lt;div id="res"&gt;&lt;/div&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">let button = document.querySelector("#load");
+button.addEventListener('click', function loadRepos() {
+   let url = 'https://api.github.com/users/testnakov/repos';
+   const httpRequest = new XMLHttpRequest();
+   httpRequest.addEventListener('readystatechange', function () {
+      if (httpRequest.readyState == 4 &amp;&amp; httpRequest.status == 200) {
+         document.getElementById("res").textContent = httpRequest.responseText;
+      }
+   });
+   httpRequest.open("GET", url);
+   httpRequest.send();
+});
+</t>
+  </si>
+  <si>
+    <t>Fetch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The fetch() method allows making network requests
+It is similar to XMLHttpRequest (XHR). The main  difference is that the Fetch API:
+Uses Promises
+Enables a simpler and cleaner API
+Makes code more readable and maintainable
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fetch('./api/some.json')
+  .then(function(response) {…})
+  .catch(function(err) {…})
+</t>
+  </si>
+  <si>
+    <t>async function getBooks() {
+    const response = await (fetch(host('books')))
+    const data = await response.json();
+    return data;
+}</t>
+  </si>
+  <si>
+    <t>Asyn/Await</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    let response = fetch(host('books'))
+        .then(resp =&gt; resp.json())
+        .then(result =&gt; result);
+    return response;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,10 +195,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -424,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,4 +534,83 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="270" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>